<commit_message>
upload in db successfully
</commit_message>
<xml_diff>
--- a/api/uploadFile/Template for upload contact.xlsx
+++ b/api/uploadFile/Template for upload contact.xlsx
@@ -1,41 +1,104 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PawanKumar\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798E1CA5-ADC5-49BC-ADD0-8646248619F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Pawan Kumar</t>
+  </si>
+  <si>
+    <t>Gautam</t>
+  </si>
+  <si>
+    <t>pawan.kumar@augtrans.com</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>faxnumber</t>
+  </si>
+  <si>
+    <t>phonenumber</t>
+  </si>
+  <si>
+    <t>contactnumber</t>
+  </si>
+  <si>
+    <t>companyname</t>
+  </si>
+  <si>
+    <t>jobprofile</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>Augmented transformations pvt ltd</t>
+  </si>
+  <si>
+    <t>full stack developer</t>
+  </si>
+  <si>
+    <t>barra</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> kanpur</t>
+  </si>
+  <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>india</t>
+  </si>
+  <si>
+    <t>google.co.uk</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,13 +128,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,151 +467,117 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>#</v>
-      </c>
-      <c r="B1" t="str">
-        <v>QR Code</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Name</v>
-      </c>
-      <c r="D1" t="str">
-        <v>email</v>
-      </c>
-      <c r="E1" t="str">
-        <v>phone1</v>
-      </c>
-      <c r="F1" t="str">
-        <v>response</v>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="str">
-        <v>Pawan Kumar</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Gautam</v>
-      </c>
-      <c r="E2" t="str">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
         <v>9625028099</v>
       </c>
-      <c r="F2" t="str">
-        <v>pawan.kumar@augtrans.com</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>2</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Rachit</v>
-      </c>
-      <c r="D3" t="str">
-        <v>Jaiswal</v>
-      </c>
-      <c r="E3" t="str">
-        <v>7985042017</v>
-      </c>
-      <c r="F3" t="str">
-        <v>rachit.jaiswal@augtrans.com</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
+      <c r="E2">
+        <v>9625028099</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="str">
-        <v>Manthan</v>
-      </c>
-      <c r="D4" t="str">
-        <v>Hebalkar</v>
-      </c>
-      <c r="E4" t="str">
-        <v>8451878825</v>
-      </c>
-      <c r="F4" t="str">
-        <v>mhebbalkar66@gmail.com</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>4</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Chaitanya</v>
-      </c>
-      <c r="D5" t="str">
-        <v>Mirpagar</v>
-      </c>
-      <c r="E5" t="str">
-        <v>8999813759</v>
-      </c>
-      <c r="F5" t="str">
-        <v>chaitanyamirpagar7261@gmail.com</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>5</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Avneesh</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Pandey</v>
-      </c>
-      <c r="E6" t="str">
-        <v>9741309162</v>
-      </c>
-      <c r="F6" t="str">
-        <v>avneesh@augtrans.com</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>6</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Demo</v>
-      </c>
-      <c r="D7" t="str">
-        <v>Contact</v>
-      </c>
-      <c r="E7" t="str">
-        <v>1234567890</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>7</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Kanchan</v>
-      </c>
-      <c r="D8" t="str">
-        <v>Nikalje</v>
-      </c>
-      <c r="E8" t="str">
-        <v>8329267597</v>
-      </c>
-      <c r="F8" t="str">
-        <v>kanchan.nikalje@orbitindia.net</v>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2">
+        <v>208001</v>
+      </c>
+      <c r="N2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F8"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>